<commit_message>
I have update the 'ensino' and 'pesquisa' sections
</commit_message>
<xml_diff>
--- a/build/ensino/2022/02/primeiro-semestre-de-2022/cronograma-mat236.xlsx
+++ b/build/ensino/2022/02/primeiro-semestre-de-2022/cronograma-mat236.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Semanas</t>
   </si>
@@ -113,22 +113,7 @@
     <t xml:space="preserve">Semana 18</t>
   </si>
   <si>
-    <t xml:space="preserve">Semana 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semana 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semana 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semana 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semana 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segunda prova</t>
+    <t>Prova</t>
   </si>
   <si>
     <t>Programa</t>
@@ -165,9 +150,6 @@
   </si>
   <si>
     <t xml:space="preserve">Trabalhos semanais.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A definir.</t>
   </si>
   <si>
     <t xml:space="preserve">Duas provas.</t>
@@ -314,10 +296,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -326,6 +311,7 @@
     <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -342,8 +328,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table1" ref="$A$1:$G$24">
-  <autoFilter ref="$A$1:$G$24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table1" ref="$A$1:$G$19">
+  <autoFilter ref="$A$1:$G$19"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Semanas"/>
     <tableColumn id="2" name="Tópico"/>
@@ -850,7 +836,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
+    <sheetView topLeftCell="C1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1143,19 +1129,19 @@
         <v>19</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" ref="C11:C24" si="4">C10+7</f>
+        <f t="shared" ref="C11:C19" si="4">C10+7</f>
         <v>44689</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:D24" si="5">D10+7</f>
+        <f t="shared" ref="D11:D19" si="5">D10+7</f>
         <v>44695</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:E24" si="6">E10+7</f>
+        <f t="shared" ref="E11:E19" si="6">E10+7</f>
         <v>44691</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F24" si="7">F10+7</f>
+        <f t="shared" ref="F11:F19" si="7">F10+7</f>
         <v>44693</v>
       </c>
       <c r="G11" s="3" t="str">
@@ -1381,163 +1367,41 @@
         <f t="shared" si="7"/>
         <v>44749</v>
       </c>
-      <c r="G19" s="3" t="str">
-        <f>Programa!$A$7</f>
-        <v xml:space="preserve">Teste de Hipóteses</v>
+      <c r="G19" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="1">
-        <f t="shared" si="4"/>
-        <v>44752</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" si="5"/>
-        <v>44758</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="6"/>
-        <v>44754</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" si="7"/>
-        <v>44756</v>
-      </c>
-      <c r="G20" s="3" t="str">
-        <f>Programa!$A$7</f>
-        <v xml:space="preserve">Teste de Hipóteses</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="1">
-        <f t="shared" si="4"/>
-        <v>44759</v>
-      </c>
-      <c r="D21" s="1">
-        <f t="shared" si="5"/>
-        <v>44765</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="6"/>
-        <v>44761</v>
-      </c>
-      <c r="F21" s="1">
-        <f t="shared" si="7"/>
-        <v>44763</v>
-      </c>
-      <c r="G21" s="3" t="str">
-        <f>Programa!$A$7</f>
-        <v xml:space="preserve">Teste de Hipóteses</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="1">
-        <f t="shared" si="4"/>
-        <v>44766</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="5"/>
-        <v>44772</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="6"/>
-        <v>44768</v>
-      </c>
-      <c r="F22" s="1">
-        <f t="shared" si="7"/>
-        <v>44770</v>
-      </c>
-      <c r="G22" s="3" t="str">
-        <f>Programa!$A$7</f>
-        <v xml:space="preserve">Teste de Hipóteses</v>
-      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="1">
-        <f t="shared" si="4"/>
-        <v>44773</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="5"/>
-        <v>44779</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" si="6"/>
-        <v>44775</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="7"/>
-        <v>44777</v>
-      </c>
-      <c r="G23" s="3" t="str">
-        <f>Programa!$A$7</f>
-        <v xml:space="preserve">Teste de Hipóteses</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="1">
-        <f t="shared" si="4"/>
-        <v>44780</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" si="5"/>
-        <v>44786</v>
-      </c>
-      <c r="E24" s="1">
-        <f t="shared" si="6"/>
-        <v>44782</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" si="7"/>
-        <v>44784</v>
-      </c>
-      <c r="G24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" s="2"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="A26" s="2"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -1564,66 +1428,66 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>39</v>
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="7">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="8">
         <v>1</v>
       </c>
       <c r="D2">
         <f>SUM(B2:B1000)</f>
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="A3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="7">
+      <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="7">
+      <c r="A5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="9">
-        <v>6</v>
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1647,35 +1511,35 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>48</v>
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>50</v>
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="8">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>50</v>
+      <c r="A3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="8">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>50</v>
+      <c r="A4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="11">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>